<commit_message>
Added python program to covert excel lists to a c string
</commit_message>
<xml_diff>
--- a/DMS-24-DEVICE_DRIVERS/TIM/TIM Throttle Map Creator/Throttle Map.xlsx
+++ b/DMS-24-DEVICE_DRIVERS/TIM/TIM Throttle Map Creator/Throttle Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FSAE\dal-fsae\DMS-24-DEVICE_DRIVERS\TIM\TIM Throttle Map Creator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8683738A-3E37-4CFD-8CB6-21995F9E3C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC14E6E4-2CC0-46F1-953A-3597315EAAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Throttle Position</t>
   </si>
@@ -54,12 +54,6 @@
   </si>
   <si>
     <t xml:space="preserve">CONTROLS </t>
-  </si>
-  <si>
-    <t>MaxVoltageOut</t>
-  </si>
-  <si>
-    <t>MinVoltageOut</t>
   </si>
   <si>
     <t>ADC Resolution</t>
@@ -90,6 +84,30 @@
   </si>
   <si>
     <t>Map D</t>
+  </si>
+  <si>
+    <t>ADC Max Bit</t>
+  </si>
+  <si>
+    <t>ThottleVoltageMax</t>
+  </si>
+  <si>
+    <t>ThottleVoltageMin</t>
+  </si>
+  <si>
+    <t>ADC Min Bit</t>
+  </si>
+  <si>
+    <t>OutputVoltageMax</t>
+  </si>
+  <si>
+    <t>OutputVoltageMin</t>
+  </si>
+  <si>
+    <t>DAC Max Bit</t>
+  </si>
+  <si>
+    <t>DAC Min Bit</t>
   </si>
 </sst>
 </file>
@@ -184,7 +202,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -192,6 +210,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -1820,13 +1839,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="93" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27:F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" customWidth="1"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="18.1796875" customWidth="1"/>
     <col min="3" max="4" width="18.7265625" customWidth="1"/>
     <col min="5" max="5" width="22.7265625" customWidth="1"/>
@@ -1840,13 +1859,20 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B2" s="4">
-        <v>3.3</v>
+        <v>3</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2">
+        <f>ROUND(B4*(B2/3.3),0)</f>
+        <v>233</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1859,13 +1885,20 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3">
+        <f>ROUND(B4*(B3/3.3),0)</f>
+        <v>0</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -1878,13 +1911,20 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" s="4">
         <v>256</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4">
+        <f>ROUND(B5*(B6/3.3),0)</f>
+        <v>4096</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1897,13 +1937,20 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4">
         <v>4096</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5">
+        <f>ROUND(B5*(B7/3.3),0)</f>
+        <v>0</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1916,12 +1963,34 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="5">
+        <v>20</v>
+      </c>
+      <c r="B6" s="7">
+        <v>3.3</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="5">
         <v>0.3</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C9" s="1"/>
@@ -2150,19 +2219,19 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
         <v>13</v>
       </c>
-      <c r="C26" t="s">
+      <c r="E26" t="s">
         <v>14</v>
       </c>
-      <c r="D26" t="s">
+      <c r="F26" t="s">
         <v>15</v>
-      </c>
-      <c r="E26" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
@@ -2170,7 +2239,23 @@
         <v>0</v>
       </c>
       <c r="B27">
-        <f>(A27*10*(($B$4-$B$3)/10))</f>
+        <f>A27*($F$2-$F$3)</f>
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <f>C12*($F$4-$F$5)</f>
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <f t="shared" ref="D27:F27" si="2">D12*($F$4-$F$5)</f>
+        <v>1228.8</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>614.4</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2179,8 +2264,24 @@
         <v>0.1</v>
       </c>
       <c r="B28">
-        <f t="shared" ref="B28:B37" si="2">(A28*10*(($B$4-$B$3)/10))</f>
-        <v>25.6</v>
+        <f t="shared" ref="B28:B37" si="3">A28*($F$2-$F$3)</f>
+        <v>23.3</v>
+      </c>
+      <c r="C28">
+        <f t="shared" ref="C28:F28" si="4">C13*($F$4-$F$5)</f>
+        <v>409.6</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="4"/>
+        <v>1515.5199999999982</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="4"/>
+        <v>819.2</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="4"/>
+        <v>102.4</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
@@ -2188,8 +2289,24 @@
         <v>0.2</v>
       </c>
       <c r="B29">
-        <f t="shared" si="2"/>
-        <v>51.2</v>
+        <f t="shared" si="3"/>
+        <v>46.6</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ref="C29:F29" si="5">C14*($F$4-$F$5)</f>
+        <v>819.2</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="5"/>
+        <v>1802.2399999999982</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="5"/>
+        <v>1024</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="5"/>
+        <v>307.2</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
@@ -2197,8 +2314,24 @@
         <v>0.3</v>
       </c>
       <c r="B30">
-        <f t="shared" si="2"/>
-        <v>76.800000000000011</v>
+        <f t="shared" si="3"/>
+        <v>69.899999999999991</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ref="C30:F30" si="6">C15*($F$4-$F$5)</f>
+        <v>1228.8</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="6"/>
+        <v>2088.9599999999982</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="6"/>
+        <v>1228.8</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="6"/>
+        <v>512</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
@@ -2206,8 +2339,24 @@
         <v>0.4</v>
       </c>
       <c r="B31">
-        <f t="shared" si="2"/>
-        <v>102.4</v>
+        <f t="shared" si="3"/>
+        <v>93.2</v>
+      </c>
+      <c r="C31">
+        <f t="shared" ref="C31:F31" si="7">C16*($F$4-$F$5)</f>
+        <v>1638.4</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="7"/>
+        <v>2375.6799999999985</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="7"/>
+        <v>1638.4000000000005</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="7"/>
+        <v>819.2</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
@@ -2215,56 +2364,174 @@
         <v>0.5</v>
       </c>
       <c r="B32">
-        <f t="shared" si="2"/>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+        <f t="shared" si="3"/>
+        <v>116.5</v>
+      </c>
+      <c r="C32">
+        <f t="shared" ref="C32:F32" si="8">C17*($F$4-$F$5)</f>
+        <v>2048</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="8"/>
+        <v>2662.3999999999987</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="8"/>
+        <v>2048.0000000000005</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="8"/>
+        <v>1228.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>0.6</v>
       </c>
       <c r="B33">
-        <f t="shared" si="2"/>
-        <v>153.60000000000002</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+        <f t="shared" si="3"/>
+        <v>139.79999999999998</v>
+      </c>
+      <c r="C33">
+        <f t="shared" ref="C33:F33" si="9">C18*($F$4-$F$5)</f>
+        <v>2457.6</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="9"/>
+        <v>2949.119999999999</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="9"/>
+        <v>2457.6000000000004</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="9"/>
+        <v>1638.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>0.7</v>
       </c>
       <c r="B34">
-        <f t="shared" si="2"/>
-        <v>179.20000000000002</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+        <f t="shared" si="3"/>
+        <v>163.1</v>
+      </c>
+      <c r="C34">
+        <f t="shared" ref="C34:F34" si="10">C19*($F$4-$F$5)</f>
+        <v>2867.2</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="10"/>
+        <v>3235.8399999999992</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="10"/>
+        <v>2867.2000000000003</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="10"/>
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>0.8</v>
       </c>
       <c r="B35">
-        <f t="shared" si="2"/>
-        <v>204.8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+        <f t="shared" si="3"/>
+        <v>186.4</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ref="C35:F35" si="11">C20*($F$4-$F$5)</f>
+        <v>3276.8</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="11"/>
+        <v>3522.5599999999995</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="11"/>
+        <v>3276.8</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="11"/>
+        <v>2457.6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>0.9</v>
       </c>
       <c r="B36">
-        <f t="shared" si="2"/>
-        <v>230.4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+        <f t="shared" si="3"/>
+        <v>209.70000000000002</v>
+      </c>
+      <c r="C36">
+        <f t="shared" ref="C36:F36" si="12">C21*($F$4-$F$5)</f>
+        <v>3686.4</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="12"/>
+        <v>3809.2799999999997</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="12"/>
+        <v>3686.4</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="12"/>
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>1</v>
       </c>
       <c r="B37">
-        <f t="shared" si="2"/>
-        <v>256</v>
+        <f t="shared" si="3"/>
+        <v>233</v>
+      </c>
+      <c r="C37">
+        <f t="shared" ref="C37:F37" si="13">C22*($F$4-$F$5)</f>
+        <v>4096</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="13"/>
+        <v>4096</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="13"/>
+        <v>4096</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="13"/>
+        <v>4096</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A26">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B11:E22">
     <cfRule type="colorScale" priority="7">
       <colorScale>
@@ -2325,30 +2592,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>